<commit_message>
Updated With new tables and added images pwrpt
</commit_message>
<xml_diff>
--- a/Mesh Convergence Study.xlsx
+++ b/Mesh Convergence Study.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecslogon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\ME7120_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Mesh Convergence Study</t>
   </si>
@@ -51,12 +52,33 @@
   </si>
   <si>
     <t>Complex Truss</t>
+  </si>
+  <si>
+    <t>Elements</t>
+  </si>
+  <si>
+    <t>Displacement (m)</t>
+  </si>
+  <si>
+    <t>Table 1: WFEM Analysis of a Non-Tapered Beam</t>
+  </si>
+  <si>
+    <t>Frequency 1 (kHz)</t>
+  </si>
+  <si>
+    <t>Frequency 2 (kHz)</t>
+  </si>
+  <si>
+    <t>Frequency 3 (kHz)</t>
+  </si>
+  <si>
+    <t>Frequency 4 (kHz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -319,11 +341,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,9 +397,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,36 +412,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,6 +421,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,6 +568,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -521,6 +620,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -675,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,32 +805,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -723,50 +839,50 @@
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -775,52 +891,52 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>1</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -829,46 +945,168 @@
       <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>1</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>5</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>10</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A2:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1.9666134765733E-2</v>
+      </c>
+      <c r="C3" s="26">
+        <v>8.2620000000000005</v>
+      </c>
+      <c r="D3" s="26">
+        <v>8.2620000000000005</v>
+      </c>
+      <c r="E3" s="26">
+        <v>81.400999999999996</v>
+      </c>
+      <c r="F3" s="31">
+        <v>81.400999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>5</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>10</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>25</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34">
+        <v>50</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Files for Report
</commit_message>
<xml_diff>
--- a/Mesh Convergence Study.xlsx
+++ b/Mesh Convergence Study.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>Mesh Convergence Study</t>
   </si>
@@ -73,13 +73,49 @@
   </si>
   <si>
     <t>Frequency 4 (kHz)</t>
+  </si>
+  <si>
+    <t>Table 2: ANSYS Analysis of a Non-Tapered Beam</t>
+  </si>
+  <si>
+    <t>Table 3: WFEM Analysis of a Tapered Beam</t>
+  </si>
+  <si>
+    <t>Table 4: ANSYS Analysis of a Non-Tapered Beam</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Table 5: Complex Orientation Max Disp.</t>
+  </si>
+  <si>
+    <t>Dof</t>
+  </si>
+  <si>
+    <t>θz</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>θx</t>
+  </si>
+  <si>
+    <t>θy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +147,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -380,11 +422,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -412,69 +480,121 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,28 +925,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -849,7 +969,7 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="17"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -857,7 +977,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
@@ -865,21 +985,21 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="18"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -901,7 +1021,7 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -911,7 +1031,7 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -919,21 +1039,21 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="18"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -955,7 +1075,7 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
@@ -963,7 +1083,7 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
@@ -971,7 +1091,7 @@
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="18"/>
+      <c r="D19" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -992,122 +1112,803 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
+      <c r="H1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="39"/>
+      <c r="K1" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="36"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="45" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="H2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
-        <v>1.9666134765733E-2</v>
-      </c>
-      <c r="C3" s="26">
+      <c r="B3" s="47">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C3" s="47">
         <v>8.2620000000000005</v>
       </c>
-      <c r="D3" s="26">
-        <v>8.2620000000000005</v>
-      </c>
-      <c r="E3" s="26">
+      <c r="D3" s="47">
         <v>81.400999999999996</v>
       </c>
-      <c r="F3" s="31">
-        <v>81.400999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
+      <c r="E3" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="13">
+        <v>-0.1993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="49">
         <v>2</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="33"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="B4" s="50">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C4" s="50">
+        <v>8.2270000000000003</v>
+      </c>
+      <c r="D4" s="50">
+        <v>51.968000000000004</v>
+      </c>
+      <c r="E4" s="50">
+        <v>175.76599999999999</v>
+      </c>
+      <c r="F4" s="51">
+        <v>510.14800000000002</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="K4" s="14">
+        <v>2</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="49">
         <v>5</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="33"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="B5" s="50">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C5" s="50">
+        <v>8.2230000000000008</v>
+      </c>
+      <c r="D5" s="50">
+        <v>51.557000000000002</v>
+      </c>
+      <c r="E5" s="50">
+        <v>144.80600000000001</v>
+      </c>
+      <c r="F5" s="51">
+        <v>286.06299999999999</v>
+      </c>
+      <c r="H5" s="14">
+        <v>5</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="K5" s="14">
+        <v>2</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="15">
+        <v>-5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="49">
         <v>10</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="33"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+      <c r="B6" s="50">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C6" s="50">
+        <v>8.2230000000000008</v>
+      </c>
+      <c r="D6" s="50">
+        <v>51.533000000000001</v>
+      </c>
+      <c r="E6" s="50">
+        <v>144.32499999999999</v>
+      </c>
+      <c r="F6" s="51">
+        <v>283.017</v>
+      </c>
+      <c r="H6" s="14">
+        <v>10</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="K6" s="14">
+        <v>2</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34">
+      <c r="M6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="49">
+        <v>25</v>
+      </c>
+      <c r="B7" s="50">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C7" s="50">
+        <v>8.2230000000000008</v>
+      </c>
+      <c r="D7" s="50">
+        <v>51.530999999999999</v>
+      </c>
+      <c r="E7" s="50">
+        <v>144.28899999999999</v>
+      </c>
+      <c r="F7" s="51">
+        <v>282.755</v>
+      </c>
+      <c r="H7" s="14">
+        <v>25</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="K7" s="14">
+        <v>2</v>
+      </c>
+      <c r="L7" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="52">
         <v>50</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="B8" s="53">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="C8" s="53">
+        <v>8.2230000000000008</v>
+      </c>
+      <c r="D8" s="53">
+        <v>51.530999999999999</v>
+      </c>
+      <c r="E8" s="53">
+        <v>144.28800000000001</v>
+      </c>
+      <c r="F8" s="54">
+        <v>282.74799999999999</v>
+      </c>
+      <c r="H8" s="16">
+        <v>50</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="K8" s="14">
+        <v>2</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="14">
+        <v>2</v>
+      </c>
+      <c r="L9" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="15">
+        <v>-0.19320000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="14">
+        <v>3</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="15">
+        <v>-8.3199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="14">
+        <v>3</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="14">
+        <v>3</v>
+      </c>
+      <c r="L13" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+      <c r="H14" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="39"/>
+      <c r="K14" s="14">
+        <v>3</v>
+      </c>
+      <c r="L14" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="14">
+        <v>3</v>
+      </c>
+      <c r="L15" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="46">
+        <v>1</v>
+      </c>
+      <c r="B16" s="47">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="C16" s="47">
+        <v>11.701000000000001</v>
+      </c>
+      <c r="D16" s="47">
+        <v>62.57</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="K16" s="14">
+        <v>4</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="49">
+        <v>2</v>
+      </c>
+      <c r="B17" s="50">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C17" s="50">
+        <v>8.6720000000000006</v>
+      </c>
+      <c r="D17" s="50">
+        <v>53.52</v>
+      </c>
+      <c r="E17" s="50">
+        <v>164.03299999999999</v>
+      </c>
+      <c r="F17" s="51">
+        <v>414.911</v>
+      </c>
+      <c r="H17" s="14">
+        <v>2</v>
+      </c>
+      <c r="I17" s="15"/>
+      <c r="K17" s="14">
+        <v>4</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="15">
+        <v>-5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="49">
+        <v>5</v>
+      </c>
+      <c r="B18" s="50">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="C18" s="50">
+        <v>7.2439999999999998</v>
+      </c>
+      <c r="D18" s="50">
+        <v>45.768999999999998</v>
+      </c>
+      <c r="E18" s="50">
+        <v>129.37899999999999</v>
+      </c>
+      <c r="F18" s="51">
+        <v>256.30500000000001</v>
+      </c>
+      <c r="H18" s="14">
+        <v>5</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="K18" s="14">
+        <v>4</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="49">
+        <v>10</v>
+      </c>
+      <c r="B19" s="50">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="C19" s="50">
+        <v>6.8639999999999999</v>
+      </c>
+      <c r="D19" s="50">
+        <v>43.115000000000002</v>
+      </c>
+      <c r="E19" s="50">
+        <v>121.03100000000001</v>
+      </c>
+      <c r="F19" s="51">
+        <v>238.00399999999999</v>
+      </c>
+      <c r="H19" s="14">
+        <v>10</v>
+      </c>
+      <c r="I19" s="15"/>
+      <c r="K19" s="14">
+        <v>4</v>
+      </c>
+      <c r="L19" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="49">
+        <v>25</v>
+      </c>
+      <c r="B20" s="50">
+        <v>4.9099999999999998E-2</v>
+      </c>
+      <c r="C20" s="50">
+        <v>6.6550000000000002</v>
+      </c>
+      <c r="D20" s="50">
+        <v>41.725000000000001</v>
+      </c>
+      <c r="E20" s="50">
+        <v>116.88</v>
+      </c>
+      <c r="F20" s="51">
+        <v>229.16</v>
+      </c>
+      <c r="H20" s="14">
+        <v>25</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="K20" s="14">
+        <v>4</v>
+      </c>
+      <c r="L20" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52">
+        <v>50</v>
+      </c>
+      <c r="B21" s="53">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="C21" s="53">
+        <v>6.5890000000000004</v>
+      </c>
+      <c r="D21" s="53">
+        <v>41.295000000000002</v>
+      </c>
+      <c r="E21" s="53">
+        <v>115.64</v>
+      </c>
+      <c r="F21" s="54">
+        <v>226.63800000000001</v>
+      </c>
+      <c r="H21" s="16">
+        <v>50</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="K21" s="14">
+        <v>4</v>
+      </c>
+      <c r="L21" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="15">
+        <v>0.19320000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="14">
+        <v>5</v>
+      </c>
+      <c r="L22" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="15">
+        <v>0.1993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="14">
+        <v>6</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="15">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="14">
+        <v>6</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="15">
+        <v>-5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="14">
+        <v>6</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="14">
+        <v>6</v>
+      </c>
+      <c r="L26" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="14">
+        <v>6</v>
+      </c>
+      <c r="L27" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="14">
+        <v>6</v>
+      </c>
+      <c r="L28" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="15">
+        <v>6.1400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="14">
+        <v>7</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K30" s="14">
+        <v>7</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="15">
+        <v>-3.4299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K31" s="14">
+        <v>7</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K32" s="14">
+        <v>7</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="14">
+        <v>7</v>
+      </c>
+      <c r="L33" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K34" s="14">
+        <v>7</v>
+      </c>
+      <c r="L34" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K35" s="14">
+        <v>8</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="15">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K36" s="14">
+        <v>8</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="15">
+        <v>-5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K37" s="14">
+        <v>8</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K38" s="14">
+        <v>8</v>
+      </c>
+      <c r="L38" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K39" s="14">
+        <v>8</v>
+      </c>
+      <c r="L39" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="11:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="16">
+        <v>8</v>
+      </c>
+      <c r="L40" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="M40" s="17">
+        <v>-6.1400000000000003E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>